<commit_message>
Created error component for error handling & Created profile-page folder for better management of styling.
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitesh Babu\Desktop\intern_project\project_torre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBD28BF8-CD71-4BB0-ADDD-6E4EF0A52EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEE115D-70FD-4740-BAEA-7B655CF4D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,39 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>4.02.2021</t>
-  </si>
-  <si>
-    <t>8:50 - 9:20</t>
-  </si>
-  <si>
-    <t>Throughly Understand API &amp; JSON fields.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:20 - 10:00 </t>
-  </si>
-  <si>
-    <t>Whiteboarded the UI.</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>Started Working on Designs.</t>
-  </si>
-  <si>
-    <t>15:00 - 16:00</t>
-  </si>
-  <si>
-    <t>Completed Search Component &amp; other UI changes for user Profile</t>
-  </si>
-  <si>
-    <t>18:00 - 18:40</t>
-  </si>
-  <si>
-    <t>Faced CORS issue, Created Proxy server in Node.js to Bypass it.</t>
-  </si>
-  <si>
     <t>5.02.2021</t>
   </si>
   <si>
@@ -92,6 +59,39 @@
   </si>
   <si>
     <t>Deployed Final Build</t>
+  </si>
+  <si>
+    <t>4.09.2021</t>
+  </si>
+  <si>
+    <t>7:30 PM - 8:00 PM</t>
+  </si>
+  <si>
+    <t>Went Through &amp; Understood API &amp; JSON fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:10 PM - 8:25 PM </t>
+  </si>
+  <si>
+    <t>8:30 PM -  10:00 PM</t>
+  </si>
+  <si>
+    <t>Project Init &amp; created some rough barebone structure to go</t>
+  </si>
+  <si>
+    <t>Did some Whiteboarding of the UI.</t>
+  </si>
+  <si>
+    <t>Completed Container &amp; Search Component.</t>
+  </si>
+  <si>
+    <t>9:00 PM - 9:30 PM</t>
+  </si>
+  <si>
+    <t>9:30 PM - 11: 00 PM</t>
+  </si>
+  <si>
+    <t>Faced CORS issue, Did some research, Created Proxy server in Node.js to Bypass it.</t>
   </si>
 </sst>
 </file>
@@ -432,13 +432,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC2D69A"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -786,13 +786,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -802,15 +802,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,6 +824,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,79 +1216,79 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.69921875" customWidth="1"/>
-    <col min="6" max="6" width="20.3984375" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
+      <c r="A1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+        <v>16</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="A4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+        <v>21</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1296,64 +1297,64 @@
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1362,40 +1363,40 @@
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+      <c r="A14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>0.60416666666666663</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1404,11 +1405,11 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1421,7 +1422,6 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
@@ -1429,6 +1429,7 @@
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Included log file & updated server file with wildcard path to match react routing & updated title in index.html
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nitesh Babu\Desktop\intern_project\project_torre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEE115D-70FD-4740-BAEA-7B655CF4D75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC63FA0-BDEE-4ED6-A995-41352DC00B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,47 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>5.02.2021</t>
-  </si>
-  <si>
-    <t>11:35 - 12:30</t>
-  </si>
-  <si>
-    <t>Worked on Profile Component.</t>
-  </si>
-  <si>
-    <t>13:00 - 13:30</t>
-  </si>
-  <si>
-    <t>Created Loading Icon</t>
-  </si>
-  <si>
-    <t>18:00 - 22:00</t>
-  </si>
-  <si>
-    <t>Worked on Card &amp; Other Components.</t>
-  </si>
-  <si>
-    <t>00:00 - 00:30</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Created Heroku Dyno for deployment &amp; Deployed for Test run.</t>
   </si>
   <si>
-    <t>6.02.2021</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
-  <si>
-    <t>Tweaked Some UI &amp; Changed Some Components</t>
-  </si>
-  <si>
-    <t>Deployed Final Build</t>
-  </si>
-  <si>
     <t>4.09.2021</t>
   </si>
   <si>
@@ -92,6 +56,72 @@
   </si>
   <si>
     <t>Faced CORS issue, Did some research, Created Proxy server in Node.js to Bypass it.</t>
+  </si>
+  <si>
+    <t>11:35 - 12:30 PM</t>
+  </si>
+  <si>
+    <t>Worked on ProfilePage &amp; Profile Component. Went Through Bootstrap.</t>
+  </si>
+  <si>
+    <t>6:00 PM - 8:00 PM</t>
+  </si>
+  <si>
+    <t>Worked on Card Designs &amp; Other Components.</t>
+  </si>
+  <si>
+    <t>5.09.2021</t>
+  </si>
+  <si>
+    <t>6.09.2021</t>
+  </si>
+  <si>
+    <t>9:00 - 10:30</t>
+  </si>
+  <si>
+    <t>10:00 PM - 11:30 PM</t>
+  </si>
+  <si>
+    <t>11: 00 - 12:30 PM</t>
+  </si>
+  <si>
+    <t>Faced some issues in commit (ENOENT : File Not Found), did some research, then used rebasing to tackle them.</t>
+  </si>
+  <si>
+    <t>7.09.2021</t>
+  </si>
+  <si>
+    <t>10:30 - 11 : 20</t>
+  </si>
+  <si>
+    <t>Worked On ProfilePic, Social Component.</t>
+  </si>
+  <si>
+    <t>Created Theme for better styling, played with some colors. Did Some UI Changes.</t>
+  </si>
+  <si>
+    <t>Created routes for Home, Profile, &amp; Job Page.</t>
+  </si>
+  <si>
+    <t>2:00 PM - 2: 30 PM</t>
+  </si>
+  <si>
+    <t>Updated Search component to use it in both Profile &amp; Job Page.</t>
+  </si>
+  <si>
+    <t>2: 40 PM - 3 : 50 PM</t>
+  </si>
+  <si>
+    <t>Worked on Job Page. Created Job Item, Job Details, Job Expectations, Job Members Page.</t>
+  </si>
+  <si>
+    <t>4 : 10 PM - 4 : 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Included Final Skills &amp; Experience Section &amp; Dropped Older Placeholder (Profile 3rd Card).</t>
+  </si>
+  <si>
+    <t>5: 00 PM - 5 : 20 PM</t>
   </si>
 </sst>
 </file>
@@ -250,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,8 +472,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -733,12 +775,110 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -786,53 +926,110 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="33" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1213,211 +1410,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="1" max="1" width="17.69921875" customWidth="1"/>
+    <col min="6" max="6" width="39.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+        <v>9</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
+      <c r="A11" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
+  <mergeCells count="23">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:F2"/>
@@ -1430,6 +1707,10 @@
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>